<commit_message>
anyadido disposable en excel, y lectura como rs
</commit_message>
<xml_diff>
--- a/data/Ventas_0002_00.xlsx
+++ b/data/Ventas_0002_00.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="28455" windowHeight="15090"/>
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -3087,9 +3087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF374"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AD374"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>

</xml_diff>